<commit_message>
may no longer need a vendor mgr
</commit_message>
<xml_diff>
--- a/DESIGN/DesignDoc.xlsx
+++ b/DESIGN/DesignDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="28035" windowHeight="11880"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="28035" windowHeight="11880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationArchitecture" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>-</t>
   </si>
@@ -125,6 +125,30 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>approval by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boon Kee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load data in application initiation and save it in termination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swarna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C(extends)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C(extends)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -589,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
@@ -611,7 +635,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -633,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -725,13 +749,13 @@
         <v>10</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="18.75">
@@ -957,7 +981,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -978,7 +1002,9 @@
       <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -998,10 +1024,19 @@
       <c r="C4" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="9">
         <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:7">

</xml_diff>